<commit_message>
Cost SU jusqu'à 7
</commit_message>
<xml_diff>
--- a/SU - Suspension/Cost/SU_A0500.xlsx
+++ b/SU - Suspension/Cost/SU_A0500.xlsx
@@ -6,7 +6,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitEPSA\SU - Suspension\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maquette_EPSA\SU - Suspension\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,77 +19,12 @@
     <sheet name="dSU 510 001" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="____________uni2">#REF!</definedName>
-    <definedName name="_________uni3">#REF!</definedName>
-    <definedName name="________uni2">#REF!</definedName>
-    <definedName name="________uni26">#REF!</definedName>
-    <definedName name="________uni4">#REF!</definedName>
-    <definedName name="________uni6">#REF!</definedName>
-    <definedName name="________uni7">#REF!</definedName>
-    <definedName name="______uni14">#REF!</definedName>
-    <definedName name="______uni54">#REF!</definedName>
-    <definedName name="_____uni3">#REF!</definedName>
-    <definedName name="____uni26">#REF!</definedName>
-    <definedName name="____uni4">#REF!</definedName>
-    <definedName name="____uni6">#REF!</definedName>
-    <definedName name="____uni7">#REF!</definedName>
-    <definedName name="___uni14">#REF!</definedName>
-    <definedName name="___uni54">#REF!</definedName>
-    <definedName name="_uni14">#REF!</definedName>
-    <definedName name="_uni2">#REF!</definedName>
-    <definedName name="_uni26">#REF!</definedName>
-    <definedName name="_uni3">#REF!</definedName>
-    <definedName name="_uni4">#REF!</definedName>
-    <definedName name="_uni54">#REF!</definedName>
-    <definedName name="_uni6">#REF!</definedName>
-    <definedName name="_uni7">#REF!</definedName>
-    <definedName name="bgtrvfcd">#REF!</definedName>
-    <definedName name="bgtvfc">#REF!</definedName>
-    <definedName name="bgvfcd">#REF!</definedName>
-    <definedName name="btgrvf">#REF!</definedName>
-    <definedName name="btvfcds">#REF!</definedName>
-    <definedName name="Car" localSheetId="0">BOM!$B$4</definedName>
-    <definedName name="Car">#REF!</definedName>
-    <definedName name="CompCode" localSheetId="0">BOM!$B$2</definedName>
-    <definedName name="CompCode">#REF!</definedName>
-    <definedName name="cwlkvclwekjc">#REF!</definedName>
-    <definedName name="dede">#REF!</definedName>
-    <definedName name="dqwdqd">#REF!</definedName>
-    <definedName name="dSU_510_001">'dSU 510 001'!$B$1</definedName>
-    <definedName name="eded">#REF!</definedName>
-    <definedName name="er">#REF!</definedName>
-    <definedName name="ervcdx">#REF!</definedName>
-    <definedName name="ezfdscx">#REF!</definedName>
-    <definedName name="gbvf">#REF!</definedName>
-    <definedName name="gbvfcd">#REF!</definedName>
-    <definedName name="gr">#REF!</definedName>
-    <definedName name="gref">#REF!</definedName>
-    <definedName name="grefzd">#REF!</definedName>
-    <definedName name="grfd">#REF!</definedName>
-    <definedName name="gtrfeds">#REF!</definedName>
-    <definedName name="gtrvfec">#REF!</definedName>
-    <definedName name="gvfc">#REF!</definedName>
-    <definedName name="gvfcd">#REF!</definedName>
-    <definedName name="gvfdc">#REF!</definedName>
-    <definedName name="hgfd">#REF!</definedName>
-    <definedName name="hygtrfvcdx">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">BOM!$6:$6</definedName>
-    <definedName name="nbtgv">#REF!</definedName>
-    <definedName name="process">#REF!</definedName>
-    <definedName name="Process_P1">#REF!</definedName>
-    <definedName name="Processes" localSheetId="0">#REF!</definedName>
-    <definedName name="Processes">#REF!</definedName>
-    <definedName name="qsfdc">#REF!</definedName>
-    <definedName name="rfcdx">#REF!</definedName>
-    <definedName name="rfds">#REF!</definedName>
-    <definedName name="rtfed">#REF!</definedName>
-    <definedName name="sdf">#REF!</definedName>
-    <definedName name="SU_510_001">'SU 510 001'!$B$6</definedName>
-    <definedName name="SU_510_001_f">'SU 510 001'!#REF!</definedName>
-    <definedName name="SU_510_001_m">'SU 510 001'!$N$12</definedName>
-    <definedName name="SU_510_001_p">'SU 510 001'!$I$22</definedName>
-    <definedName name="SU_510_001_q">'SU 510 001'!$N$3</definedName>
-    <definedName name="SU_510_001_t">'SU 510 001'!#REF!</definedName>
+    <definedName name="SU_05001">'SU 510 001'!$B$6</definedName>
+    <definedName name="SU_05001_f">'SU 510 001'!#REF!</definedName>
+    <definedName name="SU_05001_m">'SU 510 001'!$N$12</definedName>
+    <definedName name="SU_05001_p">'SU 510 001'!$I$22</definedName>
+    <definedName name="SU_05001_q">'SU 510 001'!$N$3</definedName>
+    <definedName name="SU_05001_t">'SU 510 001'!#REF!</definedName>
     <definedName name="SU_A0500">'SU A0500'!$B$5</definedName>
     <definedName name="SU_A0500_f">'SU A0500'!$J$37</definedName>
     <definedName name="SU_A0500_m">'SU A0500'!$N$18</definedName>
@@ -97,30 +32,8 @@
     <definedName name="SU_A0500_pa">'SU A0500'!$E$11</definedName>
     <definedName name="SU_A0500_q">'SU A0500'!$N$3</definedName>
     <definedName name="SU_A0500_t">'SU A0500'!$I$41</definedName>
-    <definedName name="tgfrd">#REF!</definedName>
-    <definedName name="tgrc">#REF!</definedName>
-    <definedName name="tgrf">#REF!</definedName>
-    <definedName name="tgrfcd">#REF!</definedName>
-    <definedName name="tgvrfcd">#REF!</definedName>
-    <definedName name="trfcd">#REF!</definedName>
-    <definedName name="trfds">#REF!</definedName>
-    <definedName name="trhzjyeuk">#REF!</definedName>
-    <definedName name="ujyhbgvf">#REF!</definedName>
-    <definedName name="Uni" localSheetId="0">BOM!#REF!</definedName>
-    <definedName name="Uni">#REF!</definedName>
-    <definedName name="vfcd">#REF!</definedName>
-    <definedName name="vfcdsx">#REF!</definedName>
-    <definedName name="vfdcx">#REF!</definedName>
-    <definedName name="vredcs">#REF!</definedName>
-    <definedName name="yjhtrefz">#REF!</definedName>
-    <definedName name="zaed">#REF!</definedName>
-    <definedName name="zefds">#REF!</definedName>
-    <definedName name="zefdsc">#REF!</definedName>
-    <definedName name="zefdv">#REF!</definedName>
-    <definedName name="zer">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$N$9</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -478,7 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="18">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
@@ -2207,15 +2120,15 @@
         <v>5.9234014172552163</v>
       </c>
       <c r="I8" s="124">
-        <f>SU_510_001_q</f>
+        <f>SU_05001_q</f>
         <v>2</v>
       </c>
       <c r="J8" s="125">
-        <f>SU_510_001_m</f>
+        <f>SU_05001_m</f>
         <v>0.38660141725521602</v>
       </c>
       <c r="K8" s="125">
-        <f>SU_510_001_p</f>
+        <f>SU_05001_p</f>
         <v>5.5368000000000004</v>
       </c>
       <c r="L8" s="125">
@@ -4503,7 +4416,7 @@
     <hyperlink ref="F7" location="'SU A0500'!A1" display="'SU A0500'!A1"/>
   </hyperlinks>
   <pageMargins left="0.41" right="0.22" top="0.72" bottom="0.57999999999999996" header="0.5" footer="0.26"/>
-  <pageSetup scale="61" fitToHeight="99" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="57" fitToHeight="99" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="6" max="16383" man="1"/>
@@ -4765,7 +4678,7 @@
         <v>5.9234014172552163</v>
       </c>
       <c r="D10" s="131">
-        <f>SU_510_001_q</f>
+        <f>SU_05001_q</f>
         <v>2</v>
       </c>
       <c r="E10" s="33">
@@ -5881,7 +5794,7 @@
         <v>16</v>
       </c>
       <c r="N2" s="76">
-        <f>SU_510_001_m+SU_510_001_p</f>
+        <f>SU_05001_m+SU_05001_p</f>
         <v>5.9234014172552163</v>
       </c>
       <c r="O2" s="65"/>

</xml_diff>